<commit_message>
desenhei o primeiro mapa da ala leste
</commit_message>
<xml_diff>
--- a/ala norte desenho 2.5.3.xlsx
+++ b/ala norte desenho 2.5.3.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="ala norte" sheetId="1" r:id="rId1"/>
     <sheet name="ala sul" sheetId="2" r:id="rId2"/>
-    <sheet name="ala leste final" sheetId="4" r:id="rId3"/>
-    <sheet name="nomes-numeros" sheetId="3" r:id="rId4"/>
+    <sheet name="ala leste 1" sheetId="5" r:id="rId3"/>
+    <sheet name="ala leste final" sheetId="4" r:id="rId4"/>
+    <sheet name="nomes-numeros" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>JOGADOR</t>
   </si>
@@ -136,12 +137,27 @@
   <si>
     <t>cadaveres 1</t>
   </si>
+  <si>
+    <t>porta vai pro proximo mapa 1</t>
+  </si>
+  <si>
+    <t>porta volta pro hall-ala leste</t>
+  </si>
+  <si>
+    <t>porta vai pro proximo mapa- ala leste_1    13</t>
+  </si>
+  <si>
+    <t>porta volta pro hall- ala leste 10</t>
+  </si>
+  <si>
+    <t>chave final</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,8 +213,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +337,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF990033"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -341,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -386,6 +416,10 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,6 +428,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF990033"/>
       <color rgb="FF339966"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFF9900"/>
@@ -714,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC30"/>
   <sheetViews>
-    <sheetView zoomScale="27" zoomScaleNormal="27" workbookViewId="0">
-      <selection activeCell="AY30" sqref="AY30"/>
+    <sheetView tabSelected="1" zoomScale="27" zoomScaleNormal="27" workbookViewId="0">
+      <selection activeCell="BM18" sqref="BM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,10 +975,10 @@
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
       <c r="AN5" s="2"/>
-      <c r="AR5" s="6"/>
-      <c r="AS5" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AR5" s="11"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="11"/>
+      <c r="AU5" s="11"/>
     </row>
     <row r="6" spans="1:55" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -2047,7 +2082,7 @@
   <dimension ref="A1:AY30"/>
   <sheetViews>
     <sheetView zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="AP20" sqref="AP20"/>
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3373,8 +3408,1341 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView zoomScale="31" zoomScaleNormal="31" workbookViewId="0">
+      <selection activeCell="AB17" sqref="AB17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:48" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+    </row>
+    <row r="2" spans="1:48" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="2"/>
+    </row>
+    <row r="3" spans="1:48" ht="36.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="2"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" ht="40.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="2"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+    </row>
+    <row r="6" spans="1:48" ht="36.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="2"/>
+      <c r="AS6" s="32"/>
+      <c r="AT6" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU6" s="11"/>
+      <c r="AV6" s="11"/>
+    </row>
+    <row r="7" spans="1:48" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="2"/>
+    </row>
+    <row r="8" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="2"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="2"/>
+    </row>
+    <row r="10" spans="1:48" ht="40.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="2"/>
+      <c r="AS10" s="10"/>
+      <c r="AT10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="2"/>
+    </row>
+    <row r="12" spans="1:48" ht="39" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="2"/>
+      <c r="AS12" s="11"/>
+      <c r="AT12" s="47"/>
+      <c r="AU12" s="11"/>
+      <c r="AV12" s="11"/>
+    </row>
+    <row r="13" spans="1:48" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="41"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="46"/>
+      <c r="AQ13" s="11"/>
+      <c r="AS13" s="11"/>
+    </row>
+    <row r="14" spans="1:48" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="46"/>
+    </row>
+    <row r="15" spans="1:48" ht="38.25" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A15" s="41"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="46"/>
+      <c r="AS15" s="12"/>
+      <c r="AT15" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+    </row>
+    <row r="17" spans="1:46" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="2"/>
+    </row>
+    <row r="18" spans="1:46" ht="36.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="2"/>
+      <c r="AS18" s="22"/>
+      <c r="AT18" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" ht="42.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="2"/>
+      <c r="AS19" s="45"/>
+      <c r="AT19" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="2"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="1"/>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="2"/>
+    </row>
+    <row r="21" spans="1:46" ht="38.25" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="2"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="2"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="43"/>
+      <c r="AH22" s="43"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="2"/>
+    </row>
+    <row r="23" spans="1:46" ht="40.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="43"/>
+      <c r="AH23" s="43"/>
+      <c r="AI23" s="31"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="1"/>
+      <c r="AL23" s="1"/>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="2"/>
+      <c r="AS23" s="14"/>
+      <c r="AT23" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="43"/>
+      <c r="AH24" s="43"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="2"/>
+    </row>
+    <row r="25" spans="1:46" ht="38.25" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="2"/>
+      <c r="AS25" s="11"/>
+      <c r="AT25" s="5"/>
+    </row>
+    <row r="26" spans="1:46" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="1"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="2"/>
+    </row>
+    <row r="27" spans="1:46" ht="35.25" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="2"/>
+      <c r="AS27" s="41"/>
+      <c r="AT27" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="2"/>
+    </row>
+    <row r="29" spans="1:46" ht="35.25" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="2"/>
+      <c r="AS29" s="43"/>
+      <c r="AT29" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:46" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2"/>
+      <c r="AH30" s="2"/>
+      <c r="AI30" s="2"/>
+      <c r="AJ30" s="2"/>
+      <c r="AK30" s="2"/>
+      <c r="AL30" s="2"/>
+      <c r="AM30" s="2"/>
+      <c r="AN30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AV30"/>
+  <sheetViews>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="AU26" sqref="AU26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3582,7 +4950,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
-      <c r="AE5" s="2"/>
+      <c r="AE5" s="44"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
@@ -4122,7 +5490,7 @@
       <c r="AM17" s="1"/>
       <c r="AN17" s="2"/>
     </row>
-    <row r="18" spans="1:48" ht="33.75" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:48" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" s="12"/>
@@ -4163,12 +5531,8 @@
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
-      <c r="AU18" s="22"/>
-      <c r="AV18" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:48" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:48" ht="35.25" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4209,6 +5573,10 @@
       <c r="AL19" s="1"/>
       <c r="AM19" s="1"/>
       <c r="AN19" s="2"/>
+      <c r="AU19" s="22"/>
+      <c r="AV19" s="5" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:48" ht="33.75" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A20" s="2"/>
@@ -4700,17 +6068,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -4809,7 +6177,9 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4834,7 +6204,9 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>

</xml_diff>

<commit_message>
coloquei o numero da porta do predio do tutorial na tabela
</commit_message>
<xml_diff>
--- a/ala norte desenho 2.5.3.xlsx
+++ b/ala norte desenho 2.5.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ala norte" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>JOGADOR</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>chave final</t>
+  </si>
+  <si>
+    <t>porta predio tutorial</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="27" zoomScaleNormal="27" workbookViewId="0">
+    <sheetView zoomScale="27" zoomScaleNormal="27" workbookViewId="0">
       <selection activeCell="BM18" sqref="BM18"/>
     </sheetView>
   </sheetViews>
@@ -6072,8 +6075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6213,7 +6216,9 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>

</xml_diff>